<commit_message>
Updated Summary of Contributions
</commit_message>
<xml_diff>
--- a/Documentation/Summary_of_Contributions.xlsx
+++ b/Documentation/Summary_of_Contributions.xlsx
@@ -5,20 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\Dal Coursework\Winter_2022\CSCI 5308\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\Dal Coursework\Winter_2022\CSCI 5308\SPRING PROJECT\group16\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DDB737-47CD-49FC-89D9-14FD16B181D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F0E0B7-DA2C-4848-8D7F-8A98D83F5AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C8D53F86-0B4F-434D-91A6-1822D6878DA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{C8D53F86-0B4F-434D-91A6-1822D6878DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Contributions" sheetId="1" r:id="rId1"/>
-    <sheet name="GitLab" sheetId="5" r:id="rId2"/>
+    <sheet name="GitLab" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="JIRA" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2669,8 +2668,8 @@
   </sheetPr>
   <dimension ref="A1:Q297"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6302,8 +6301,8 @@
   </sheetPr>
   <dimension ref="A1:BS35"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BS4" sqref="BS4"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BQ4" sqref="BQ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>